<commit_message>
Corrección: Verificacion del Identificador
</commit_message>
<xml_diff>
--- a/Tabla Error.xlsx
+++ b/Tabla Error.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +478,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>@</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>7</v>
@@ -510,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C6" t="n">
         <v>7</v>
@@ -526,14 +526,14 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -542,14 +542,14 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>@</t>
         </is>
       </c>
     </row>
@@ -558,14 +558,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>$</t>
         </is>
       </c>
     </row>
@@ -574,14 +574,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>”</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -590,14 +590,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>”</t>
         </is>
       </c>
     </row>
@@ -606,12 +606,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
+        <v>146</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
         <v>150</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>12</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>@</t>
         </is>

</xml_diff>

<commit_message>
Validacion Ruta: 24 validaciones finalizada.
</commit_message>
<xml_diff>
--- a/Tabla Error.xlsx
+++ b/Tabla Error.xlsx
@@ -690,7 +690,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>fin</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>fin</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>fin</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -722,7 +722,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>fin</t>
         </is>
       </c>
     </row>
@@ -732,7 +732,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -743,7 +743,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
     </row>
@@ -753,18 +753,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
     </row>
@@ -774,18 +774,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>peso</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>peso</t>
         </is>
       </c>
     </row>
@@ -795,18 +795,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>peso</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>peso</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -827,7 +827,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -848,7 +848,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección: Identificador de ruta.
</commit_message>
<xml_diff>
--- a/Tabla Error.xlsx
+++ b/Tabla Error.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +478,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
-      </c>
-      <c r="C4" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>I</t>
+          <t xml:space="preserve">	</t>
         </is>
       </c>
     </row>
@@ -494,14 +491,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
         <v>22</v>
       </c>
-      <c r="C5" t="n">
-        <v>7</v>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>@</t>
         </is>
       </c>
     </row>
@@ -510,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
         <v>7</v>
@@ -526,14 +523,14 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -542,14 +539,14 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>I</t>
         </is>
       </c>
     </row>
@@ -558,14 +555,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>@</t>
         </is>
       </c>
     </row>
@@ -574,14 +571,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>137</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>”</t>
+          <t>$</t>
         </is>
       </c>
     </row>
@@ -590,7 +587,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="C11" t="n">
         <v>7</v>
@@ -606,12 +603,44 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
+        <v>137</v>
+      </c>
+      <c r="C12" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>”</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>146</v>
+      </c>
+      <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
         <v>150</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C14" t="n">
         <v>12</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>@</t>
         </is>
@@ -690,18 +719,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
     </row>
@@ -711,7 +740,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -722,7 +751,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>fin</t>
+          <t>nombre</t>
         </is>
       </c>
     </row>
@@ -732,7 +761,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>fin</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -743,7 +772,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>fin</t>
         </is>
       </c>
     </row>
@@ -753,7 +782,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>fin</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -764,7 +793,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>inicio</t>
+          <t>fin</t>
         </is>
       </c>
     </row>
@@ -774,7 +803,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -785,7 +814,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
     </row>
@@ -795,18 +824,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>peso</t>
+          <t>inicio</t>
         </is>
       </c>
     </row>
@@ -816,18 +845,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>peso</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
         <v>6</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>peso</t>
         </is>
       </c>
     </row>
@@ -837,18 +866,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>peso</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>nombre</t>
+          <t>peso</t>
         </is>
       </c>
     </row>

</xml_diff>